<commit_message>
Completed Cost Estimator page
</commit_message>
<xml_diff>
--- a/addact/public/redirects.xlsx
+++ b/addact/public/redirects.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="631">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
     <t>source</t>
   </si>
@@ -2361,17 +2361,17 @@
   <dimension ref="A1:C331"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A317" workbookViewId="0">
-      <selection activeCell="A333" sqref="A333"/>
+      <selection activeCell="C331" sqref="C331" activeCellId="0"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="107.44140625" customWidth="1"/>
     <col min="2" max="2" width="83.109375" customWidth="1"/>
     <col min="3" max="3" width="14.21875" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" customFormat="1" s="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2382,7 +2382,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2">
       <c r="A2" s="8" t="s">
         <v>14</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3">
       <c r="A3" s="8" t="s">
         <v>16</v>
       </c>
@@ -2404,7 +2404,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4">
       <c r="A4" s="8" t="s">
         <v>18</v>
       </c>
@@ -2415,7 +2415,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5">
       <c r="A5" s="8" t="s">
         <v>20</v>
       </c>
@@ -2426,7 +2426,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6">
       <c r="A6" s="8" t="s">
         <v>22</v>
       </c>
@@ -2437,7 +2437,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7">
       <c r="A7" s="8" t="s">
         <v>24</v>
       </c>
@@ -2448,7 +2448,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8">
       <c r="A8" s="8" t="s">
         <v>26</v>
       </c>
@@ -2459,7 +2459,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9">
       <c r="A9" s="8" t="s">
         <v>28</v>
       </c>
@@ -2470,7 +2470,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10">
       <c r="A10" s="8" t="s">
         <v>30</v>
       </c>
@@ -2481,7 +2481,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11">
       <c r="A11" s="8" t="s">
         <v>32</v>
       </c>
@@ -2492,7 +2492,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12">
       <c r="A12" s="8" t="s">
         <v>34</v>
       </c>
@@ -2503,7 +2503,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13">
       <c r="A13" s="8" t="s">
         <v>35</v>
       </c>
@@ -2514,7 +2514,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14">
       <c r="A14" s="8" t="s">
         <v>37</v>
       </c>
@@ -2525,7 +2525,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15">
       <c r="A15" s="8" t="s">
         <v>39</v>
       </c>
@@ -2536,7 +2536,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16">
       <c r="A16" s="8" t="s">
         <v>41</v>
       </c>
@@ -2547,7 +2547,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17">
       <c r="A17" s="8" t="s">
         <v>43</v>
       </c>
@@ -2558,7 +2558,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18">
       <c r="A18" s="8" t="s">
         <v>45</v>
       </c>
@@ -2569,7 +2569,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19">
       <c r="A19" s="8" t="s">
         <v>47</v>
       </c>
@@ -2580,7 +2580,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20">
       <c r="A20" s="8" t="s">
         <v>49</v>
       </c>
@@ -2591,7 +2591,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21">
       <c r="A21" s="8" t="s">
         <v>51</v>
       </c>
@@ -2602,7 +2602,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22">
       <c r="A22" s="8" t="s">
         <v>53</v>
       </c>
@@ -2613,7 +2613,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23">
       <c r="A23" s="8" t="s">
         <v>55</v>
       </c>
@@ -2624,7 +2624,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24">
       <c r="A24" s="8" t="s">
         <v>57</v>
       </c>
@@ -2635,7 +2635,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25">
       <c r="A25" s="8" t="s">
         <v>59</v>
       </c>
@@ -2646,7 +2646,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26">
       <c r="A26" s="8" t="s">
         <v>61</v>
       </c>
@@ -2657,7 +2657,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27">
       <c r="A27" s="8" t="s">
         <v>63</v>
       </c>
@@ -2668,7 +2668,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28">
       <c r="A28" s="8" t="s">
         <v>65</v>
       </c>
@@ -2679,7 +2679,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29">
       <c r="A29" s="8" t="s">
         <v>67</v>
       </c>
@@ -2690,7 +2690,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30">
       <c r="A30" s="8" t="s">
         <v>69</v>
       </c>
@@ -2701,7 +2701,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31">
       <c r="A31" s="8" t="s">
         <v>71</v>
       </c>
@@ -2712,7 +2712,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32">
       <c r="A32" s="8" t="s">
         <v>73</v>
       </c>
@@ -2723,7 +2723,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33">
       <c r="A33" s="8" t="s">
         <v>75</v>
       </c>
@@ -2734,7 +2734,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34">
       <c r="A34" s="8" t="s">
         <v>77</v>
       </c>
@@ -2745,7 +2745,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35">
       <c r="A35" s="8" t="s">
         <v>79</v>
       </c>
@@ -2756,7 +2756,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36">
       <c r="A36" s="8" t="s">
         <v>81</v>
       </c>
@@ -2767,7 +2767,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37">
       <c r="A37" s="8" t="s">
         <v>83</v>
       </c>
@@ -2778,7 +2778,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38">
       <c r="A38" s="8" t="s">
         <v>85</v>
       </c>
@@ -2789,7 +2789,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39">
       <c r="A39" s="8" t="s">
         <v>87</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40">
       <c r="A40" s="8" t="s">
         <v>89</v>
       </c>
@@ -2811,7 +2811,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41">
       <c r="A41" s="8" t="s">
         <v>91</v>
       </c>
@@ -2822,7 +2822,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42">
       <c r="A42" s="8" t="s">
         <v>93</v>
       </c>
@@ -2833,7 +2833,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="43" ht="27">
       <c r="A43" s="9" t="s">
         <v>95</v>
       </c>
@@ -2844,7 +2844,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44">
       <c r="A44" s="8" t="s">
         <v>97</v>
       </c>
@@ -2855,7 +2855,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45">
       <c r="A45" s="8" t="s">
         <v>99</v>
       </c>
@@ -2866,7 +2866,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46">
       <c r="A46" s="8" t="s">
         <v>101</v>
       </c>
@@ -2877,7 +2877,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47">
       <c r="A47" s="8" t="s">
         <v>103</v>
       </c>
@@ -2888,7 +2888,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48">
       <c r="A48" s="8" t="s">
         <v>105</v>
       </c>
@@ -2899,7 +2899,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49">
       <c r="A49" s="8" t="s">
         <v>107</v>
       </c>
@@ -2910,7 +2910,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50">
       <c r="A50" s="8" t="s">
         <v>109</v>
       </c>
@@ -2921,7 +2921,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51">
       <c r="A51" s="8" t="s">
         <v>111</v>
       </c>
@@ -2932,7 +2932,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52">
       <c r="A52" s="8" t="s">
         <v>113</v>
       </c>
@@ -2943,7 +2943,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53">
       <c r="A53" s="8" t="s">
         <v>115</v>
       </c>
@@ -2954,7 +2954,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54">
       <c r="A54" s="8" t="s">
         <v>117</v>
       </c>
@@ -2965,7 +2965,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55">
       <c r="A55" s="8" t="s">
         <v>119</v>
       </c>
@@ -2976,7 +2976,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56">
       <c r="A56" s="8" t="s">
         <v>121</v>
       </c>
@@ -2987,7 +2987,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57">
       <c r="A57" s="8" t="s">
         <v>123</v>
       </c>
@@ -2998,7 +2998,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58">
       <c r="A58" s="8" t="s">
         <v>125</v>
       </c>
@@ -3009,7 +3009,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59">
       <c r="A59" s="8" t="s">
         <v>127</v>
       </c>
@@ -3020,7 +3020,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60">
       <c r="A60" s="8" t="s">
         <v>129</v>
       </c>
@@ -3031,7 +3031,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61">
       <c r="A61" s="8" t="s">
         <v>131</v>
       </c>
@@ -3042,7 +3042,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62">
       <c r="A62" s="8" t="s">
         <v>133</v>
       </c>
@@ -3053,7 +3053,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63">
       <c r="A63" s="8" t="s">
         <v>135</v>
       </c>
@@ -3064,7 +3064,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="64" ht="27">
       <c r="A64" s="9" t="s">
         <v>137</v>
       </c>
@@ -3075,7 +3075,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65">
       <c r="A65" s="8" t="s">
         <v>139</v>
       </c>
@@ -3086,7 +3086,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66">
       <c r="A66" s="8" t="s">
         <v>141</v>
       </c>
@@ -3097,7 +3097,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67">
       <c r="A67" s="8" t="s">
         <v>143</v>
       </c>
@@ -3108,7 +3108,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68">
       <c r="A68" s="8" t="s">
         <v>145</v>
       </c>
@@ -3119,7 +3119,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69">
       <c r="A69" s="8" t="s">
         <v>147</v>
       </c>
@@ -3130,7 +3130,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70">
       <c r="A70" s="8" t="s">
         <v>149</v>
       </c>
@@ -3141,7 +3141,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="71" ht="27">
       <c r="A71" s="9" t="s">
         <v>151</v>
       </c>
@@ -3152,7 +3152,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="72" ht="27">
       <c r="A72" s="9" t="s">
         <v>153</v>
       </c>
@@ -3163,7 +3163,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73">
       <c r="A73" s="8" t="s">
         <v>155</v>
       </c>
@@ -3174,7 +3174,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74">
       <c r="A74" s="8" t="s">
         <v>157</v>
       </c>
@@ -3185,7 +3185,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="75" ht="27">
       <c r="A75" s="9" t="s">
         <v>159</v>
       </c>
@@ -3196,7 +3196,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76">
       <c r="A76" s="8" t="s">
         <v>161</v>
       </c>
@@ -3207,7 +3207,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77">
       <c r="A77" s="8" t="s">
         <v>163</v>
       </c>
@@ -3218,7 +3218,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78">
       <c r="A78" s="8" t="s">
         <v>165</v>
       </c>
@@ -3229,7 +3229,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79">
       <c r="A79" s="8" t="s">
         <v>167</v>
       </c>
@@ -3240,7 +3240,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80">
       <c r="A80" s="8" t="s">
         <v>169</v>
       </c>
@@ -3251,7 +3251,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81">
       <c r="A81" s="8" t="s">
         <v>171</v>
       </c>
@@ -3262,7 +3262,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82">
       <c r="A82" s="8" t="s">
         <v>173</v>
       </c>
@@ -3273,7 +3273,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83">
       <c r="A83" s="8" t="s">
         <v>175</v>
       </c>
@@ -3284,7 +3284,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84">
       <c r="A84" s="8" t="s">
         <v>177</v>
       </c>
@@ -3295,7 +3295,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85">
       <c r="A85" s="8" t="s">
         <v>179</v>
       </c>
@@ -3306,7 +3306,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86">
       <c r="A86" s="8" t="s">
         <v>181</v>
       </c>
@@ -3317,7 +3317,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87">
       <c r="A87" s="8" t="s">
         <v>183</v>
       </c>
@@ -3328,7 +3328,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88">
       <c r="A88" s="8" t="s">
         <v>185</v>
       </c>
@@ -3339,7 +3339,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89">
       <c r="A89" s="8" t="s">
         <v>187</v>
       </c>
@@ -3350,7 +3350,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90">
       <c r="A90" s="8" t="s">
         <v>189</v>
       </c>
@@ -3361,7 +3361,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91">
       <c r="A91" s="8" t="s">
         <v>191</v>
       </c>
@@ -3372,7 +3372,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92">
       <c r="A92" s="8" t="s">
         <v>193</v>
       </c>
@@ -3383,7 +3383,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93">
       <c r="A93" s="8" t="s">
         <v>195</v>
       </c>
@@ -3394,7 +3394,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94">
       <c r="A94" s="8" t="s">
         <v>197</v>
       </c>
@@ -3405,7 +3405,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="95" ht="27">
       <c r="A95" s="9" t="s">
         <v>199</v>
       </c>
@@ -3416,7 +3416,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96">
       <c r="A96" s="8" t="s">
         <v>201</v>
       </c>
@@ -3427,7 +3427,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97">
       <c r="A97" s="8" t="s">
         <v>203</v>
       </c>
@@ -3438,7 +3438,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98">
       <c r="A98" s="8" t="s">
         <v>205</v>
       </c>
@@ -3449,7 +3449,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="99" ht="27">
       <c r="A99" s="9" t="s">
         <v>207</v>
       </c>
@@ -3460,7 +3460,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100">
       <c r="A100" s="8" t="s">
         <v>209</v>
       </c>
@@ -3471,7 +3471,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101">
       <c r="A101" s="8" t="s">
         <v>211</v>
       </c>
@@ -3482,7 +3482,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102">
       <c r="A102" s="8" t="s">
         <v>213</v>
       </c>
@@ -3493,7 +3493,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="103">
       <c r="A103" s="8" t="s">
         <v>215</v>
       </c>
@@ -3504,7 +3504,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="104">
       <c r="A104" s="8" t="s">
         <v>217</v>
       </c>
@@ -3515,7 +3515,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="105">
       <c r="A105" s="8" t="s">
         <v>219</v>
       </c>
@@ -3526,7 +3526,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106">
       <c r="A106" s="8" t="s">
         <v>221</v>
       </c>
@@ -3537,7 +3537,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="107">
       <c r="A107" s="8" t="s">
         <v>223</v>
       </c>
@@ -3548,7 +3548,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="108">
       <c r="A108" s="8" t="s">
         <v>225</v>
       </c>
@@ -3559,7 +3559,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="109">
       <c r="A109" s="8" t="s">
         <v>227</v>
       </c>
@@ -3570,7 +3570,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="110">
       <c r="A110" s="8" t="s">
         <v>229</v>
       </c>
@@ -3581,7 +3581,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111">
       <c r="A111" s="8" t="s">
         <v>231</v>
       </c>
@@ -3592,7 +3592,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112">
       <c r="A112" s="8" t="s">
         <v>233</v>
       </c>
@@ -3603,7 +3603,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="113">
       <c r="A113" s="8" t="s">
         <v>235</v>
       </c>
@@ -3614,7 +3614,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="114">
       <c r="A114" s="8" t="s">
         <v>237</v>
       </c>
@@ -3625,7 +3625,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="115">
       <c r="A115" s="8" t="s">
         <v>239</v>
       </c>
@@ -3636,7 +3636,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="116">
       <c r="A116" s="8" t="s">
         <v>241</v>
       </c>
@@ -3647,7 +3647,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="117" ht="27">
       <c r="A117" s="9" t="s">
         <v>243</v>
       </c>
@@ -3658,7 +3658,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="118">
       <c r="A118" s="8" t="s">
         <v>245</v>
       </c>
@@ -3669,7 +3669,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="119">
       <c r="A119" s="8" t="s">
         <v>247</v>
       </c>
@@ -3680,7 +3680,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="120">
       <c r="A120" s="8" t="s">
         <v>249</v>
       </c>
@@ -3691,7 +3691,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="121">
       <c r="A121" s="8" t="s">
         <v>251</v>
       </c>
@@ -3702,7 +3702,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="122" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="122" ht="27">
       <c r="A122" s="9" t="s">
         <v>253</v>
       </c>
@@ -3713,7 +3713,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="123">
       <c r="A123" s="8" t="s">
         <v>255</v>
       </c>
@@ -3724,7 +3724,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="124">
       <c r="A124" s="8" t="s">
         <v>257</v>
       </c>
@@ -3735,7 +3735,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="125">
       <c r="A125" s="8" t="s">
         <v>259</v>
       </c>
@@ -3746,7 +3746,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="126">
       <c r="A126" s="8" t="s">
         <v>261</v>
       </c>
@@ -3757,7 +3757,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="127">
       <c r="A127" s="8" t="s">
         <v>263</v>
       </c>
@@ -3768,7 +3768,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="128">
       <c r="A128" s="8" t="s">
         <v>265</v>
       </c>
@@ -3779,7 +3779,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="129">
       <c r="A129" s="8" t="s">
         <v>267</v>
       </c>
@@ -3790,7 +3790,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="130">
       <c r="A130" s="8" t="s">
         <v>269</v>
       </c>
@@ -3801,7 +3801,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="131">
       <c r="A131" s="8" t="s">
         <v>271</v>
       </c>
@@ -3812,7 +3812,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="132">
       <c r="A132" s="8" t="s">
         <v>273</v>
       </c>
@@ -3823,7 +3823,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="133">
       <c r="A133" s="8" t="s">
         <v>275</v>
       </c>
@@ -3834,7 +3834,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="134">
       <c r="A134" s="8" t="s">
         <v>277</v>
       </c>
@@ -3845,7 +3845,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="135">
       <c r="A135" s="8" t="s">
         <v>279</v>
       </c>
@@ -3856,7 +3856,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="136">
       <c r="A136" s="8" t="s">
         <v>281</v>
       </c>
@@ -3867,7 +3867,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="137">
       <c r="A137" s="8" t="s">
         <v>283</v>
       </c>
@@ -3878,7 +3878,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="138">
       <c r="A138" s="8" t="s">
         <v>285</v>
       </c>
@@ -3889,7 +3889,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="139" ht="27">
       <c r="A139" s="9" t="s">
         <v>287</v>
       </c>
@@ -3900,7 +3900,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="140">
       <c r="A140" s="8" t="s">
         <v>289</v>
       </c>
@@ -3911,7 +3911,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="141">
       <c r="A141" s="8" t="s">
         <v>291</v>
       </c>
@@ -3922,7 +3922,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="142">
       <c r="A142" s="8" t="s">
         <v>293</v>
       </c>
@@ -3933,7 +3933,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="143">
       <c r="A143" s="8" t="s">
         <v>295</v>
       </c>
@@ -3944,7 +3944,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="144">
       <c r="A144" s="8" t="s">
         <v>297</v>
       </c>
@@ -3955,7 +3955,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="145">
       <c r="A145" s="8" t="s">
         <v>299</v>
       </c>
@@ -3966,7 +3966,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="146">
       <c r="A146" s="8" t="s">
         <v>301</v>
       </c>
@@ -3977,7 +3977,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="147">
       <c r="A147" s="8" t="s">
         <v>303</v>
       </c>
@@ -3988,7 +3988,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="148">
       <c r="A148" s="8" t="s">
         <v>305</v>
       </c>
@@ -3999,7 +3999,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="149">
       <c r="A149" s="8" t="s">
         <v>307</v>
       </c>
@@ -4010,7 +4010,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="150">
       <c r="A150" s="8" t="s">
         <v>309</v>
       </c>
@@ -4021,7 +4021,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="151">
       <c r="A151" s="8" t="s">
         <v>311</v>
       </c>
@@ -4032,7 +4032,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="152">
       <c r="A152" s="8" t="s">
         <v>313</v>
       </c>
@@ -4043,7 +4043,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="153">
       <c r="A153" s="8" t="s">
         <v>315</v>
       </c>
@@ -4054,7 +4054,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="154">
       <c r="A154" s="8" t="s">
         <v>317</v>
       </c>
@@ -4065,7 +4065,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="155">
       <c r="A155" s="8" t="s">
         <v>319</v>
       </c>
@@ -4076,7 +4076,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="156">
       <c r="A156" s="8" t="s">
         <v>321</v>
       </c>
@@ -4087,7 +4087,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="157">
       <c r="A157" s="8" t="s">
         <v>323</v>
       </c>
@@ -4098,7 +4098,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="158">
       <c r="A158" s="8" t="s">
         <v>325</v>
       </c>
@@ -4109,7 +4109,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="159">
       <c r="A159" s="8" t="s">
         <v>327</v>
       </c>
@@ -4120,7 +4120,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="160">
       <c r="A160" s="8" t="s">
         <v>329</v>
       </c>
@@ -4131,7 +4131,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="161">
       <c r="A161" s="8" t="s">
         <v>331</v>
       </c>
@@ -4142,7 +4142,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="162">
       <c r="A162" s="8" t="s">
         <v>333</v>
       </c>
@@ -4153,7 +4153,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="163">
       <c r="A163" s="8" t="s">
         <v>335</v>
       </c>
@@ -4164,7 +4164,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="164">
       <c r="A164" s="8" t="s">
         <v>337</v>
       </c>
@@ -4175,7 +4175,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="165">
       <c r="A165" s="8" t="s">
         <v>339</v>
       </c>
@@ -4186,7 +4186,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="166">
       <c r="A166" s="8" t="s">
         <v>341</v>
       </c>
@@ -4197,7 +4197,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="167">
       <c r="A167" s="8" t="s">
         <v>343</v>
       </c>
@@ -4208,7 +4208,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="168">
       <c r="A168" s="8" t="s">
         <v>345</v>
       </c>
@@ -4219,7 +4219,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="169">
       <c r="A169" s="8" t="s">
         <v>347</v>
       </c>
@@ -4230,7 +4230,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="170">
       <c r="A170" s="8" t="s">
         <v>349</v>
       </c>
@@ -4241,7 +4241,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="171">
       <c r="A171" s="8" t="s">
         <v>351</v>
       </c>
@@ -4252,7 +4252,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="172">
       <c r="A172" s="8" t="s">
         <v>353</v>
       </c>
@@ -4263,7 +4263,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="173">
       <c r="A173" s="8" t="s">
         <v>355</v>
       </c>
@@ -4274,7 +4274,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="174">
       <c r="A174" s="8" t="s">
         <v>357</v>
       </c>
@@ -4285,7 +4285,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="175">
       <c r="A175" s="8" t="s">
         <v>359</v>
       </c>
@@ -4296,7 +4296,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="176">
       <c r="A176" s="8" t="s">
         <v>361</v>
       </c>
@@ -4307,7 +4307,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="177">
       <c r="A177" s="8" t="s">
         <v>363</v>
       </c>
@@ -4318,7 +4318,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="178">
       <c r="A178" s="8" t="s">
         <v>365</v>
       </c>
@@ -4329,7 +4329,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="179">
       <c r="A179" s="8" t="s">
         <v>367</v>
       </c>
@@ -4340,7 +4340,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="180">
       <c r="A180" s="8" t="s">
         <v>369</v>
       </c>
@@ -4351,7 +4351,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="181">
       <c r="A181" s="8" t="s">
         <v>371</v>
       </c>
@@ -4362,7 +4362,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="182">
       <c r="A182" s="8" t="s">
         <v>373</v>
       </c>
@@ -4373,7 +4373,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="183" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="183" ht="42">
       <c r="A183" s="9" t="s">
         <v>375</v>
       </c>
@@ -4384,7 +4384,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="184">
       <c r="A184" s="8" t="s">
         <v>377</v>
       </c>
@@ -4395,7 +4395,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="185">
       <c r="A185" s="8" t="s">
         <v>379</v>
       </c>
@@ -4406,7 +4406,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="186">
       <c r="A186" s="8" t="s">
         <v>381</v>
       </c>
@@ -4417,7 +4417,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="187">
       <c r="A187" s="8" t="s">
         <v>383</v>
       </c>
@@ -4428,7 +4428,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="188">
       <c r="A188" s="8" t="s">
         <v>385</v>
       </c>
@@ -4439,7 +4439,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="189">
       <c r="A189" s="8" t="s">
         <v>387</v>
       </c>
@@ -4450,7 +4450,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="190">
       <c r="A190" s="8" t="s">
         <v>389</v>
       </c>
@@ -4461,7 +4461,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="191">
       <c r="A191" s="8" t="s">
         <v>391</v>
       </c>
@@ -4472,7 +4472,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="192">
       <c r="A192" s="8" t="s">
         <v>393</v>
       </c>
@@ -4483,7 +4483,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="193">
       <c r="A193" s="8" t="s">
         <v>395</v>
       </c>
@@ -4494,7 +4494,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="194">
       <c r="A194" s="8" t="s">
         <v>397</v>
       </c>
@@ -4505,7 +4505,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="195">
       <c r="A195" s="8" t="s">
         <v>399</v>
       </c>
@@ -4516,7 +4516,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="196">
       <c r="A196" s="8" t="s">
         <v>401</v>
       </c>
@@ -4527,7 +4527,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="197">
       <c r="A197" s="8" t="s">
         <v>403</v>
       </c>
@@ -4538,7 +4538,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="198">
       <c r="A198" s="8" t="s">
         <v>405</v>
       </c>
@@ -4549,7 +4549,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="199">
       <c r="A199" s="8" t="s">
         <v>407</v>
       </c>
@@ -4560,7 +4560,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="200">
       <c r="A200" s="8" t="s">
         <v>409</v>
       </c>
@@ -4571,7 +4571,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="201">
       <c r="A201" s="8" t="s">
         <v>411</v>
       </c>
@@ -4582,7 +4582,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="202">
       <c r="A202" s="8" t="s">
         <v>413</v>
       </c>
@@ -4593,7 +4593,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="203">
       <c r="A203" s="8" t="s">
         <v>415</v>
       </c>
@@ -4604,7 +4604,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="204">
       <c r="A204" s="8" t="s">
         <v>417</v>
       </c>
@@ -4615,7 +4615,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="205">
       <c r="A205" s="8" t="s">
         <v>419</v>
       </c>
@@ -4626,7 +4626,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="206">
       <c r="A206" s="8" t="s">
         <v>421</v>
       </c>
@@ -4637,7 +4637,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="207">
       <c r="A207" s="8" t="s">
         <v>423</v>
       </c>
@@ -4648,7 +4648,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="208">
       <c r="A208" s="8" t="s">
         <v>425</v>
       </c>
@@ -4659,7 +4659,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="209">
       <c r="A209" s="8" t="s">
         <v>427</v>
       </c>
@@ -4670,7 +4670,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="210" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="210" ht="27">
       <c r="A210" s="9" t="s">
         <v>429</v>
       </c>
@@ -4681,7 +4681,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="211">
       <c r="A211" s="8" t="s">
         <v>431</v>
       </c>
@@ -4692,7 +4692,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="212">
       <c r="A212" s="8" t="s">
         <v>433</v>
       </c>
@@ -4703,7 +4703,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="213">
       <c r="A213" s="8" t="s">
         <v>435</v>
       </c>
@@ -4714,7 +4714,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="214">
       <c r="A214" s="8" t="s">
         <v>437</v>
       </c>
@@ -4725,7 +4725,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="215">
       <c r="A215" s="8" t="s">
         <v>439</v>
       </c>
@@ -4736,7 +4736,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="216">
       <c r="A216" s="8" t="s">
         <v>441</v>
       </c>
@@ -4747,7 +4747,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="217">
       <c r="A217" s="8" t="s">
         <v>443</v>
       </c>
@@ -4758,7 +4758,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="218">
       <c r="A218" s="8" t="s">
         <v>445</v>
       </c>
@@ -4769,7 +4769,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="219">
       <c r="A219" s="8" t="s">
         <v>446</v>
       </c>
@@ -4780,7 +4780,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="220">
       <c r="A220" s="8" t="s">
         <v>448</v>
       </c>
@@ -4791,7 +4791,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="221">
       <c r="A221" s="8" t="s">
         <v>450</v>
       </c>
@@ -4802,7 +4802,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="222">
       <c r="A222" s="8" t="s">
         <v>452</v>
       </c>
@@ -4813,7 +4813,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="223">
       <c r="A223" s="8" t="s">
         <v>454</v>
       </c>
@@ -4824,7 +4824,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="224">
       <c r="A224" s="8" t="s">
         <v>456</v>
       </c>
@@ -4835,7 +4835,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="225">
       <c r="A225" s="8" t="s">
         <v>458</v>
       </c>
@@ -4846,7 +4846,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="226">
       <c r="A226" s="8" t="s">
         <v>460</v>
       </c>
@@ -4857,7 +4857,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="227">
       <c r="A227" s="8" t="s">
         <v>462</v>
       </c>
@@ -4868,7 +4868,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="228">
       <c r="A228" s="8" t="s">
         <v>464</v>
       </c>
@@ -4879,7 +4879,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="229">
       <c r="A229" s="8" t="s">
         <v>466</v>
       </c>
@@ -4890,7 +4890,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="230">
       <c r="A230" s="8" t="s">
         <v>468</v>
       </c>
@@ -4901,7 +4901,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="231">
       <c r="A231" s="8" t="s">
         <v>470</v>
       </c>
@@ -4912,7 +4912,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="232">
       <c r="A232" s="8" t="s">
         <v>472</v>
       </c>
@@ -4923,7 +4923,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="233">
       <c r="A233" s="8" t="s">
         <v>474</v>
       </c>
@@ -4934,7 +4934,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="234">
       <c r="A234" s="8" t="s">
         <v>476</v>
       </c>
@@ -4945,7 +4945,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="235">
       <c r="A235" s="8" t="s">
         <v>478</v>
       </c>
@@ -4956,7 +4956,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="236">
       <c r="A236" s="8" t="s">
         <v>480</v>
       </c>
@@ -4967,7 +4967,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="237" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="237" ht="42">
       <c r="A237" s="9" t="s">
         <v>482</v>
       </c>
@@ -4978,7 +4978,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="238">
       <c r="A238" s="8" t="s">
         <v>484</v>
       </c>
@@ -4989,7 +4989,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="239">
       <c r="A239" s="8" t="s">
         <v>486</v>
       </c>
@@ -5000,7 +5000,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="240" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="240" ht="27">
       <c r="A240" s="9" t="s">
         <v>488</v>
       </c>
@@ -5011,7 +5011,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="241">
       <c r="A241" s="8" t="s">
         <v>490</v>
       </c>
@@ -5022,7 +5022,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="242">
       <c r="A242" s="8" t="s">
         <v>492</v>
       </c>
@@ -5033,7 +5033,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="243">
       <c r="A243" s="8" t="s">
         <v>494</v>
       </c>
@@ -5044,7 +5044,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="244">
       <c r="A244" s="8" t="s">
         <v>496</v>
       </c>
@@ -5055,7 +5055,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="245" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="245" ht="42">
       <c r="A245" s="9" t="s">
         <v>498</v>
       </c>
@@ -5066,7 +5066,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="246">
       <c r="A246" s="8" t="s">
         <v>500</v>
       </c>
@@ -5077,7 +5077,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="247" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="247" ht="42">
       <c r="A247" s="9" t="s">
         <v>502</v>
       </c>
@@ -5088,7 +5088,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="248">
       <c r="A248" s="8" t="s">
         <v>504</v>
       </c>
@@ -5099,7 +5099,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="249">
       <c r="A249" s="8" t="s">
         <v>506</v>
       </c>
@@ -5110,7 +5110,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="250" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="250" ht="27">
       <c r="A250" s="9" t="s">
         <v>508</v>
       </c>
@@ -5121,7 +5121,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="251" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="251" ht="42">
       <c r="A251" s="9" t="s">
         <v>510</v>
       </c>
@@ -5132,7 +5132,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="252">
       <c r="A252" s="8" t="s">
         <v>512</v>
       </c>
@@ -5143,7 +5143,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="253">
       <c r="A253" s="8" t="s">
         <v>514</v>
       </c>
@@ -5154,7 +5154,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="254">
       <c r="A254" s="8" t="s">
         <v>516</v>
       </c>
@@ -5165,7 +5165,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="255">
       <c r="A255" s="8" t="s">
         <v>518</v>
       </c>
@@ -5176,7 +5176,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="256" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="256" ht="27">
       <c r="A256" s="9" t="s">
         <v>520</v>
       </c>
@@ -5187,7 +5187,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="257">
       <c r="A257" s="8" t="s">
         <v>522</v>
       </c>
@@ -5198,7 +5198,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="258">
       <c r="A258" s="8" t="s">
         <v>524</v>
       </c>
@@ -5209,7 +5209,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="259">
       <c r="A259" s="8" t="s">
         <v>526</v>
       </c>
@@ -5220,7 +5220,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="260">
       <c r="A260" s="8" t="s">
         <v>528</v>
       </c>
@@ -5231,7 +5231,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="261">
       <c r="A261" s="8" t="s">
         <v>530</v>
       </c>
@@ -5242,7 +5242,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="262">
       <c r="A262" s="8" t="s">
         <v>532</v>
       </c>
@@ -5253,7 +5253,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="263">
       <c r="A263" s="8" t="s">
         <v>534</v>
       </c>
@@ -5264,7 +5264,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="264">
       <c r="A264" s="8" t="s">
         <v>536</v>
       </c>
@@ -5275,7 +5275,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="265">
       <c r="A265" s="8" t="s">
         <v>538</v>
       </c>
@@ -5286,7 +5286,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="266">
       <c r="A266" s="8" t="s">
         <v>540</v>
       </c>
@@ -5297,7 +5297,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="267">
       <c r="A267" s="8" t="s">
         <v>542</v>
       </c>
@@ -5308,7 +5308,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="268">
       <c r="A268" s="8" t="s">
         <v>544</v>
       </c>
@@ -5319,7 +5319,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="269">
       <c r="A269" s="8" t="s">
         <v>546</v>
       </c>
@@ -5330,7 +5330,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="270">
       <c r="A270" s="8" t="s">
         <v>548</v>
       </c>
@@ -5341,7 +5341,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="271">
       <c r="A271" s="8" t="s">
         <v>550</v>
       </c>
@@ -5352,7 +5352,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="272">
       <c r="A272" s="8" t="s">
         <v>552</v>
       </c>
@@ -5363,7 +5363,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="273">
       <c r="A273" s="8" t="s">
         <v>554</v>
       </c>
@@ -5374,7 +5374,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="274">
       <c r="A274" s="8" t="s">
         <v>556</v>
       </c>
@@ -5385,7 +5385,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="275">
       <c r="A275" s="8" t="s">
         <v>558</v>
       </c>
@@ -5396,7 +5396,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="276" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="276" ht="27">
       <c r="A276" s="9" t="s">
         <v>560</v>
       </c>
@@ -5407,7 +5407,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="277">
       <c r="A277" s="8" t="s">
         <v>562</v>
       </c>
@@ -5418,7 +5418,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="278">
       <c r="A278" s="8" t="s">
         <v>564</v>
       </c>
@@ -5429,7 +5429,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="279">
       <c r="A279" s="8" t="s">
         <v>566</v>
       </c>
@@ -5440,7 +5440,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="280" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="280" ht="27">
       <c r="A280" s="9" t="s">
         <v>568</v>
       </c>
@@ -5451,7 +5451,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="281">
       <c r="A281" s="8" t="s">
         <v>570</v>
       </c>
@@ -5462,7 +5462,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="282">
       <c r="A282" s="8" t="s">
         <v>572</v>
       </c>
@@ -5473,7 +5473,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="283">
       <c r="A283" s="9" t="s">
         <v>574</v>
       </c>
@@ -5484,7 +5484,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="284">
       <c r="A284" s="8" t="s">
         <v>576</v>
       </c>
@@ -5495,7 +5495,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="285" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="285" ht="27">
       <c r="A285" s="9" t="s">
         <v>578</v>
       </c>
@@ -5506,7 +5506,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="286">
       <c r="A286" s="3" t="s">
         <v>7</v>
       </c>
@@ -5517,7 +5517,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="287">
       <c r="A287" s="3" t="s">
         <v>4</v>
       </c>
@@ -5528,7 +5528,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="288">
       <c r="A288" s="3" t="s">
         <v>11</v>
       </c>
@@ -5539,7 +5539,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="289">
       <c r="A289" s="3" t="s">
         <v>6</v>
       </c>
@@ -5550,7 +5550,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="290">
       <c r="A290" s="3" t="s">
         <v>9</v>
       </c>
@@ -5561,7 +5561,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="291">
       <c r="A291" s="3" t="s">
         <v>5</v>
       </c>
@@ -5572,7 +5572,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="292">
       <c r="A292" s="3" t="s">
         <v>10</v>
       </c>
@@ -5583,7 +5583,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="293">
       <c r="A293" s="3" t="s">
         <v>8</v>
       </c>
@@ -5594,7 +5594,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="294">
       <c r="A294" s="3" t="s">
         <v>587</v>
       </c>
@@ -5605,7 +5605,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="295" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="295" ht="27">
       <c r="A295" s="2" t="s">
         <v>589</v>
       </c>
@@ -5616,7 +5616,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="296" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="296" ht="27">
       <c r="A296" s="2" t="s">
         <v>591</v>
       </c>
@@ -5627,7 +5627,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="297" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="297" ht="27">
       <c r="A297" s="2" t="s">
         <v>593</v>
       </c>
@@ -5638,7 +5638,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="298" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="298" ht="27">
       <c r="A298" s="2" t="s">
         <v>574</v>
       </c>
@@ -5649,7 +5649,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="299">
       <c r="A299" s="3" t="s">
         <v>576</v>
       </c>
@@ -5660,7 +5660,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="300" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="300" ht="27">
       <c r="A300" s="2" t="s">
         <v>578</v>
       </c>
@@ -5671,7 +5671,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="301">
       <c r="A301" s="3" t="s">
         <v>595</v>
       </c>
@@ -5682,7 +5682,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="302">
       <c r="A302" s="3" t="s">
         <v>596</v>
       </c>
@@ -5693,7 +5693,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="303">
       <c r="A303" s="3" t="s">
         <v>597</v>
       </c>
@@ -5704,7 +5704,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="304">
       <c r="A304" s="3" t="s">
         <v>598</v>
       </c>
@@ -5715,7 +5715,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="305">
       <c r="A305" s="3" t="s">
         <v>599</v>
       </c>
@@ -5726,7 +5726,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="306">
       <c r="A306" s="3" t="s">
         <v>600</v>
       </c>
@@ -5737,7 +5737,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="307">
       <c r="A307" s="3" t="s">
         <v>601</v>
       </c>
@@ -5748,7 +5748,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="308">
       <c r="A308" s="3" t="s">
         <v>602</v>
       </c>
@@ -5759,7 +5759,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="309">
       <c r="A309" s="3" t="s">
         <v>603</v>
       </c>
@@ -5770,7 +5770,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="310">
       <c r="A310" s="3" t="s">
         <v>604</v>
       </c>
@@ -5781,7 +5781,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="311">
       <c r="A311" s="3" t="s">
         <v>605</v>
       </c>
@@ -5792,7 +5792,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="312">
       <c r="A312" s="3" t="s">
         <v>607</v>
       </c>
@@ -5803,7 +5803,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="313">
       <c r="A313" s="3" t="s">
         <v>608</v>
       </c>
@@ -5814,7 +5814,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="314">
       <c r="A314" s="3" t="s">
         <v>609</v>
       </c>
@@ -5825,7 +5825,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="315">
       <c r="A315" s="3" t="s">
         <v>611</v>
       </c>
@@ -5836,7 +5836,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="316">
       <c r="A316" s="3" t="s">
         <v>613</v>
       </c>
@@ -5847,7 +5847,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="317">
       <c r="A317" s="3" t="s">
         <v>614</v>
       </c>
@@ -5858,7 +5858,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="318" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="318">
       <c r="A318" s="3" t="s">
         <v>615</v>
       </c>
@@ -5869,7 +5869,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="319">
       <c r="A319" s="3" t="s">
         <v>616</v>
       </c>
@@ -5880,7 +5880,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="320">
       <c r="A320" s="3" t="s">
         <v>617</v>
       </c>
@@ -5891,7 +5891,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="321" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="321">
       <c r="A321" s="3" t="s">
         <v>618</v>
       </c>
@@ -5902,7 +5902,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="322" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="322">
       <c r="A322" s="3" t="s">
         <v>619</v>
       </c>
@@ -5913,7 +5913,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="323" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="323">
       <c r="A323" s="3" t="s">
         <v>620</v>
       </c>
@@ -5924,7 +5924,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="324" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="324">
       <c r="A324" s="3" t="s">
         <v>621</v>
       </c>
@@ -5935,7 +5935,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="325" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="325">
       <c r="A325" s="3" t="s">
         <v>623</v>
       </c>
@@ -5946,7 +5946,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="326" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="326">
       <c r="A326" s="11" t="s">
         <v>620</v>
       </c>
@@ -5957,7 +5957,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="327" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="327">
       <c r="A327" s="11" t="s">
         <v>621</v>
       </c>
@@ -5968,7 +5968,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="328" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="328">
       <c r="A328" s="11" t="s">
         <v>623</v>
       </c>
@@ -5979,7 +5979,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="329" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="329">
       <c r="A329" s="10" t="s">
         <v>445</v>
       </c>
@@ -5990,27 +5990,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="330" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="330">
       <c r="A330" s="10" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="B330" s="10" t="s">
-        <v>625</v>
+        <v>629</v>
       </c>
       <c r="C330" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="331" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A331" s="10" t="s">
-        <v>628</v>
-      </c>
-      <c r="B331" s="10" t="s">
-        <v>629</v>
-      </c>
-      <c r="C331" s="6" t="s">
-        <v>3</v>
-      </c>
+    <row r="331">
+      <c r="C331" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>